<commit_message>
changed appsetings access levels
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hiv_treatment_verification.xlsx
+++ b/config/default/forms/app/hiv_treatment_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\hivTreatment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64534044-3331-457D-9EBA-583963FEB4D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E4DFA2-B1FD-4F68-952A-3A46C1E66746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="81585" yWindow="2715" windowWidth="6000" windowHeight="2985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="83250" yWindow="7215" windowWidth="6000" windowHeight="2985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="202">
   <si>
     <t>type</t>
   </si>
@@ -247,9 +247,6 @@
     <t>Is a PEPFAR site?</t>
   </si>
   <si>
-    <t>HIV Monitoring</t>
-  </si>
-  <si>
     <t>facility_name</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
     <t>levels</t>
   </si>
   <si>
-    <t>Levels:</t>
-  </si>
-  <si>
     <t>disclosed_status</t>
   </si>
   <si>
@@ -331,15 +325,9 @@
     <t>IPT</t>
   </si>
   <si>
-    <t>Month and Year started IPT:</t>
-  </si>
-  <si>
     <t>when_initiated_on_treatment</t>
   </si>
   <si>
-    <t>Month and Year initiated on OI treatment:</t>
-  </si>
-  <si>
     <t>care_model</t>
   </si>
   <si>
@@ -382,15 +370,6 @@
     <t>when_diagnosed_with_oi</t>
   </si>
   <si>
-    <t>Month and Year diagnosed with OI:</t>
-  </si>
-  <si>
-    <t>Month and Year completed OI treatment:</t>
-  </si>
-  <si>
-    <t>Month and Year Initiated OI treatment:</t>
-  </si>
-  <si>
     <t>Comments:</t>
   </si>
   <si>
@@ -448,9 +427,6 @@
     <t>opportunistic_infections</t>
   </si>
   <si>
-    <t xml:space="preserve">Candididiasis </t>
-  </si>
-  <si>
     <t>Cryptococcosis</t>
   </si>
   <si>
@@ -508,9 +484,6 @@
     <t>Single Drug Substitution</t>
   </si>
   <si>
-    <t xml:space="preserve"> Baseline VL</t>
-  </si>
-  <si>
     <t>baselinevl</t>
   </si>
   <si>
@@ -548,6 +521,126 @@
   </si>
   <si>
     <t>${to_who}=”other”</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Count:</t>
+  </si>
+  <si>
+    <t>Baseline VL</t>
+  </si>
+  <si>
+    <t>${supprot_group}=”yes”</t>
+  </si>
+  <si>
+    <t>Candididiasis</t>
+  </si>
+  <si>
+    <t>Cytomegalovisus Infection (CMV)</t>
+  </si>
+  <si>
+    <t>cytomegalovisus</t>
+  </si>
+  <si>
+    <t>Herpes Zoster</t>
+  </si>
+  <si>
+    <t>herpes</t>
+  </si>
+  <si>
+    <t>HIV Encephalitis</t>
+  </si>
+  <si>
+    <t>HIV_encephalitis</t>
+  </si>
+  <si>
+    <t>Kaposi sarcoma</t>
+  </si>
+  <si>
+    <t>kaposi_sarcoma</t>
+  </si>
+  <si>
+    <t>Pneumonystis carinii pneumonia</t>
+  </si>
+  <si>
+    <t>pneumonystis_carinii_pneumonia</t>
+  </si>
+  <si>
+    <t>Toxoplasmosis</t>
+  </si>
+  <si>
+    <t>Tuberculosis</t>
+  </si>
+  <si>
+    <t>toxoplasmosis</t>
+  </si>
+  <si>
+    <t>tuberculosis</t>
+  </si>
+  <si>
+    <t>Other (Specify)</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>CD4 Count</t>
+  </si>
+  <si>
+    <t>select_one source_of_info</t>
+  </si>
+  <si>
+    <t>source_of_info</t>
+  </si>
+  <si>
+    <t>verbal_report</t>
+  </si>
+  <si>
+    <t>Verbal Report</t>
+  </si>
+  <si>
+    <t>appointment_card</t>
+  </si>
+  <si>
+    <t>Appointment Card</t>
+  </si>
+  <si>
+    <t>phone_call_written_record</t>
+  </si>
+  <si>
+    <t>Phone Call Written record</t>
+  </si>
+  <si>
+    <t>sms</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>eid_dashboard</t>
+  </si>
+  <si>
+    <t>EID Dashboard</t>
+  </si>
+  <si>
+    <t>Date diagnosed:</t>
+  </si>
+  <si>
+    <t>Date initiated OI treatment:</t>
+  </si>
+  <si>
+    <t>Date completed OI treatment:</t>
+  </si>
+  <si>
+    <t>Date started IPT:</t>
+  </si>
+  <si>
+    <t>Date completed IPT:</t>
   </si>
 </sst>
 </file>
@@ -655,7 +748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -694,9 +787,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -710,232 +800,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB7B7B7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="90">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF980000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB7B7B7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB7B7B7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -961,6 +830,395 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB7B7B7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB7B7B7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB7B7B7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB7B7B7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB7B7B7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9EAD3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1777,13 +2035,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y77"/>
+  <dimension ref="A1:Y76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E63" sqref="E63"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2683,10 +2941,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -2753,13 +3011,13 @@
         <v>50</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -2788,13 +3046,13 @@
         <v>54</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -2820,10 +3078,10 @@
     </row>
     <row r="31" spans="1:25" ht="13.5">
       <c r="A31" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>69</v>
@@ -2858,10 +3116,10 @@
         <v>50</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -2891,10 +3149,10 @@
         <v>54</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="8"/>
@@ -2921,16 +3179,16 @@
     </row>
     <row r="34" spans="1:25" ht="13.5">
       <c r="A34" s="5" t="s">
-        <v>54</v>
+        <v>185</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -3042,10 +3300,10 @@
         <v>13</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>70</v>
+        <v>184</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -3077,10 +3335,10 @@
         <v>50</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>57</v>
@@ -3112,13 +3370,13 @@
         <v>54</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -3257,10 +3515,10 @@
         <v>13</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -3292,13 +3550,13 @@
         <v>50</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -3324,16 +3582,16 @@
     </row>
     <row r="47" spans="1:25" ht="13.5">
       <c r="A47" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="D47" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -3362,13 +3620,13 @@
         <v>54</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -3394,16 +3652,16 @@
     </row>
     <row r="49" spans="1:25" ht="13.5">
       <c r="A49" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="5"/>
@@ -3429,17 +3687,17 @@
     </row>
     <row r="50" spans="1:25" ht="13.5">
       <c r="A50" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="8" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
@@ -3467,14 +3725,14 @@
         <v>54</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
@@ -3585,10 +3843,10 @@
         <v>13</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
@@ -3620,13 +3878,13 @@
         <v>50</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>98</v>
+        <v>200</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -3655,13 +3913,13 @@
         <v>50</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>100</v>
+        <v>201</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -3719,10 +3977,10 @@
         <v>13</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -3751,16 +4009,16 @@
     </row>
     <row r="62" spans="1:25" ht="13.5">
       <c r="A62" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -3786,16 +4044,16 @@
     </row>
     <row r="63" spans="1:25" ht="13.5">
       <c r="A63" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
@@ -3824,15 +4082,17 @@
         <v>54</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E64" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>166</v>
+      </c>
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
@@ -3915,10 +4175,10 @@
         <v>13</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
@@ -3947,13 +4207,13 @@
     </row>
     <row r="69" spans="1:25" ht="27">
       <c r="A69" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>57</v>
@@ -3981,49 +4241,49 @@
       <c r="Y69" s="5"/>
     </row>
     <row r="70" spans="1:25" ht="13.5">
-      <c r="A70" s="17" t="s">
+      <c r="A70" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="D70" s="17"/>
+      <c r="B70" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D70" s="16"/>
       <c r="E70" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
-      <c r="J70" s="17"/>
-      <c r="K70" s="17"/>
-      <c r="L70" s="17"/>
-      <c r="M70" s="17"/>
-      <c r="N70" s="17"/>
-      <c r="O70" s="17"/>
-      <c r="P70" s="17"/>
-      <c r="Q70" s="17"/>
-      <c r="R70" s="17"/>
-      <c r="S70" s="17"/>
-      <c r="T70" s="17"/>
-      <c r="U70" s="17"/>
-      <c r="V70" s="17"/>
-      <c r="W70" s="17"/>
-      <c r="X70" s="17"/>
-      <c r="Y70" s="17"/>
+        <v>156</v>
+      </c>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
+      <c r="K70" s="16"/>
+      <c r="L70" s="16"/>
+      <c r="M70" s="16"/>
+      <c r="N70" s="16"/>
+      <c r="O70" s="16"/>
+      <c r="P70" s="16"/>
+      <c r="Q70" s="16"/>
+      <c r="R70" s="16"/>
+      <c r="S70" s="16"/>
+      <c r="T70" s="16"/>
+      <c r="U70" s="16"/>
+      <c r="V70" s="16"/>
+      <c r="W70" s="16"/>
+      <c r="X70" s="16"/>
+      <c r="Y70" s="16"/>
     </row>
     <row r="71" spans="1:25" ht="13.5">
       <c r="A71" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>57</v>
@@ -4051,14 +4311,14 @@
       <c r="Y71" s="5"/>
     </row>
     <row r="72" spans="1:25" ht="13.5">
-      <c r="A72" s="14" t="s">
+      <c r="A72" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B72" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C72" s="14" t="s">
-        <v>116</v>
+      <c r="B72" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>57</v>
@@ -4086,14 +4346,14 @@
       <c r="Y72" s="5"/>
     </row>
     <row r="73" spans="1:25" ht="13.5">
-      <c r="A73" s="14" t="s">
+      <c r="A73" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B73" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C73" s="14" t="s">
-        <v>117</v>
+      <c r="B73" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>57</v>
@@ -4122,19 +4382,21 @@
     </row>
     <row r="74" spans="1:25" ht="13.5">
       <c r="A74" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D74" s="5"/>
+        <v>112</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
@@ -4154,22 +4416,14 @@
       <c r="Y74" s="5"/>
     </row>
     <row r="75" spans="1:25" ht="13.5">
-      <c r="A75" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
@@ -4189,7 +4443,9 @@
       <c r="Y75" s="5"/>
     </row>
     <row r="76" spans="1:25" ht="13.5">
-      <c r="A76" s="5"/>
+      <c r="A76" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -4215,380 +4471,437 @@
       <c r="X76" s="5"/>
       <c r="Y76" s="5"/>
     </row>
-    <row r="77" spans="1:25" ht="13.5">
-      <c r="A77" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
-      <c r="M77" s="5"/>
-      <c r="N77" s="5"/>
-      <c r="O77" s="5"/>
-      <c r="P77" s="5"/>
-      <c r="Q77" s="5"/>
-      <c r="R77" s="5"/>
-      <c r="S77" s="5"/>
-      <c r="T77" s="5"/>
-      <c r="U77" s="5"/>
-      <c r="V77" s="5"/>
-      <c r="W77" s="5"/>
-      <c r="X77" s="5"/>
-      <c r="Y77" s="5"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Y49 A74:Y994 A52:Y67 A50:D51 F50:Y51">
-    <cfRule type="containsText" dxfId="71" priority="98" operator="containsText" text="calculate"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y49 A74:Y979 A52:Y67 A50:D51 F50:Y51">
-    <cfRule type="expression" dxfId="70" priority="99">
+  <conditionalFormatting sqref="A1:Y33 A52:Y63 A50:D51 F50:Y51 A65:Y67 A64:D64 F64:Y64 A35:Y49 A74:Y993">
+    <cfRule type="containsText" dxfId="89" priority="116" operator="containsText" text="calculate"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:Y33 A52:Y63 A50:D51 F50:Y51 A65:Y67 A64:D64 F64:Y64 A35:Y49 A74:Y978">
+    <cfRule type="expression" dxfId="88" priority="117">
       <formula>AND($A1="begin group", NOT($B1 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y49 A74:Y994 A52:Y67 A50:D51 F50:Y51">
-    <cfRule type="expression" dxfId="69" priority="100">
+  <conditionalFormatting sqref="A1:Y33 A52:Y63 A50:D51 F50:Y51 A65:Y67 A64:D64 F64:Y64 A35:Y49 A74:Y993">
+    <cfRule type="expression" dxfId="87" priority="118">
       <formula>AND($A1="end group", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $L1 = "", $M1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y49 A74:Y994 A52:Y67 A50:D51 F50:Y51">
-    <cfRule type="cellIs" dxfId="68" priority="101" operator="equal">
+  <conditionalFormatting sqref="A1:Y33 A52:Y63 A50:D51 F50:Y51 A65:Y67 A64:D64 F64:Y64 A35:Y49 A74:Y993">
+    <cfRule type="cellIs" dxfId="86" priority="119" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I67 I74:I994">
-    <cfRule type="expression" dxfId="67" priority="104">
+  <conditionalFormatting sqref="I1:I33 I35:I67 I74:I993">
+    <cfRule type="expression" dxfId="85" priority="122">
       <formula>AND($I1 = "", $A1 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C67 C74:C994">
-    <cfRule type="expression" dxfId="66" priority="105">
+  <conditionalFormatting sqref="C1:C33 C35:C67 C74:C993">
+    <cfRule type="expression" dxfId="84" priority="123">
       <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $C1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B67 B74:B994">
-    <cfRule type="expression" dxfId="65" priority="106">
+  <conditionalFormatting sqref="B1:B33 B35:B67 B74:B993">
+    <cfRule type="expression" dxfId="83" priority="124">
       <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $B1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A67 A74:A994">
-    <cfRule type="cellIs" dxfId="64" priority="107" operator="equal">
+  <conditionalFormatting sqref="A1:A33 A35:A67 A74:A993">
+    <cfRule type="cellIs" dxfId="82" priority="125" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" dxfId="63" priority="109" operator="notEqual">
+    <cfRule type="cellIs" dxfId="81" priority="127" operator="notEqual">
       <formula>"name"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsText" dxfId="62" priority="110" operator="notContains" text="label"/>
+    <cfRule type="notContainsText" dxfId="80" priority="128" operator="notContains" text="label"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" dxfId="61" priority="111" operator="notEqual">
+    <cfRule type="cellIs" dxfId="79" priority="129" operator="notEqual">
       <formula>"required"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="60" priority="112" operator="notEqual">
+    <cfRule type="cellIs" dxfId="78" priority="130" operator="notEqual">
       <formula>"relevant"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="59" priority="113" operator="notEqual">
+    <cfRule type="cellIs" dxfId="77" priority="131" operator="notEqual">
       <formula>"appearance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="58" priority="114" operator="notEqual">
+    <cfRule type="cellIs" dxfId="76" priority="132" operator="notEqual">
       <formula>"constraint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="notContainsText" dxfId="57" priority="115" operator="notContains" text="constraint_message"/>
+    <cfRule type="notContainsText" dxfId="75" priority="133" operator="notContains" text="constraint_message"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" dxfId="56" priority="116" operator="notEqual">
+    <cfRule type="cellIs" dxfId="74" priority="134" operator="notEqual">
       <formula>"calculation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="55" priority="117" operator="notEqual">
+    <cfRule type="cellIs" dxfId="73" priority="135" operator="notEqual">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" dxfId="54" priority="118" operator="notContains" text="hint"/>
+    <cfRule type="notContainsText" dxfId="72" priority="136" operator="notContains" text="hint"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" dxfId="53" priority="119" operator="notEqual">
+    <cfRule type="cellIs" dxfId="71" priority="137" operator="notEqual">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" dxfId="52" priority="120" operator="notEqual">
+    <cfRule type="cellIs" dxfId="70" priority="138" operator="notEqual">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H67 H74:H979">
-    <cfRule type="expression" dxfId="51" priority="121">
+  <conditionalFormatting sqref="H1:H33 H35:H67 H74:H978">
+    <cfRule type="expression" dxfId="69" priority="139">
       <formula>AND(NOT($G1 = ""), $H1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y49 A74:Y979 A52:Y67 A50:D51 F50:Y51">
-    <cfRule type="expression" dxfId="50" priority="122">
+  <conditionalFormatting sqref="A1:Y33 A52:Y63 A50:D51 F50:Y51 A65:Y67 A64:D64 F64:Y64 A35:Y49 A74:Y978">
+    <cfRule type="expression" dxfId="68" priority="140">
       <formula>AND($A1="begin repeat", NOT($B1 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y49 A74:Y994 A52:Y67 A50:D51 F50:Y51">
-    <cfRule type="expression" dxfId="49" priority="123">
+  <conditionalFormatting sqref="A1:Y33 A52:Y63 A50:D51 F50:Y51 A65:Y67 A64:D64 F64:Y64 A35:Y49 A74:Y993">
+    <cfRule type="expression" dxfId="67" priority="141">
       <formula>AND($A1="end repeat", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $L1 = "", $M1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:Y69 A71:Y72">
-    <cfRule type="containsText" dxfId="48" priority="37" operator="containsText" text="calculate"/>
+    <cfRule type="containsText" dxfId="66" priority="55" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:Y69 A71:Y72">
-    <cfRule type="expression" dxfId="47" priority="38">
+    <cfRule type="expression" dxfId="65" priority="56">
       <formula>AND($A68="begin group", NOT($B68 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:Y69 A71:Y72">
-    <cfRule type="expression" dxfId="46" priority="39">
+    <cfRule type="expression" dxfId="64" priority="57">
       <formula>AND($A68="end group", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:Y69 A71:Y72">
-    <cfRule type="cellIs" dxfId="45" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="58" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I68:I69 I71:I72">
-    <cfRule type="expression" dxfId="44" priority="41">
+    <cfRule type="expression" dxfId="62" priority="59">
       <formula>AND($I68 = "", $A68 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C69 C71:C72">
-    <cfRule type="expression" dxfId="43" priority="42">
+    <cfRule type="expression" dxfId="61" priority="60">
       <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $C68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68:B69 B71:B72">
-    <cfRule type="expression" dxfId="42" priority="43">
+    <cfRule type="expression" dxfId="60" priority="61">
       <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $B68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:A69 A71:A72">
-    <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:H69 H71:H72">
-    <cfRule type="expression" dxfId="40" priority="45">
+    <cfRule type="expression" dxfId="58" priority="63">
       <formula>AND(NOT($G68 = ""), $H68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:Y69 A71:Y72">
-    <cfRule type="expression" dxfId="39" priority="46">
+    <cfRule type="expression" dxfId="57" priority="64">
       <formula>AND($A68="begin repeat", NOT($B68 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:Y69 A71:Y72">
-    <cfRule type="expression" dxfId="38" priority="47">
+    <cfRule type="expression" dxfId="56" priority="65">
       <formula>AND($A68="end repeat", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73:Y73">
-    <cfRule type="containsText" dxfId="37" priority="25" operator="containsText" text="calculate"/>
+    <cfRule type="containsText" dxfId="55" priority="43" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73:Y73">
-    <cfRule type="expression" dxfId="36" priority="26">
+    <cfRule type="expression" dxfId="54" priority="44">
       <formula>AND($A73="begin group", NOT($B73 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73:Y73">
-    <cfRule type="expression" dxfId="35" priority="27">
+    <cfRule type="expression" dxfId="53" priority="45">
       <formula>AND($A73="end group", $B73 = "", $C73 = "", $D73 = "", $E73 = "", $F73 = "", $G73 = "", $H73 = "", $I73 = "", $J73 = "", $K73 = "", $L73 = "", $M73 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73:Y73">
-    <cfRule type="cellIs" dxfId="34" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="46" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="33" priority="29">
+    <cfRule type="expression" dxfId="51" priority="47">
       <formula>AND($I73 = "", $A73 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73">
-    <cfRule type="expression" dxfId="32" priority="30">
+    <cfRule type="expression" dxfId="50" priority="48">
       <formula>AND(AND(NOT($A73 = "end group"), NOT($A73 = "end repeat"), NOT($A73 = "")), $C73 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="expression" dxfId="31" priority="31">
+    <cfRule type="expression" dxfId="49" priority="49">
       <formula>AND(AND(NOT($A73 = "end group"), NOT($A73 = "end repeat"), NOT($A73 = "")), $B73 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73">
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73">
-    <cfRule type="expression" dxfId="29" priority="33">
+    <cfRule type="expression" dxfId="47" priority="51">
       <formula>AND(NOT($G73 = ""), $H73 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73:Y73">
-    <cfRule type="expression" dxfId="28" priority="34">
+    <cfRule type="expression" dxfId="46" priority="52">
       <formula>AND($A73="begin repeat", NOT($B73 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73:Y73">
-    <cfRule type="expression" dxfId="27" priority="35">
+    <cfRule type="expression" dxfId="45" priority="53">
       <formula>AND($A73="end repeat", $B73 = "", $C73 = "", $D73 = "", $E73 = "", $F73 = "", $G73 = "", $H73 = "", $I73 = "", $J73 = "", $K73 = "", $L73 = "", $M73 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B69 B71:B987">
-    <cfRule type="expression" dxfId="26" priority="331">
-      <formula>COUNTIF($B$2:$B$987,B2)&gt;1</formula>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="containsText" dxfId="44" priority="37" operator="containsText" text="calculate"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="expression" dxfId="43" priority="38">
+      <formula>AND($A50="begin group", NOT($B50 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="expression" dxfId="42" priority="39">
+      <formula>AND($A50="end group", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="expression" dxfId="40" priority="41">
+      <formula>AND($A50="begin repeat", NOT($B50 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="expression" dxfId="39" priority="42">
+      <formula>AND($A50="end repeat", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:Y70">
+    <cfRule type="containsText" dxfId="38" priority="25" operator="containsText" text="calculate"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:Y70">
+    <cfRule type="expression" dxfId="37" priority="26">
+      <formula>AND($A70="begin group", NOT($B70 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:Y70">
+    <cfRule type="expression" dxfId="36" priority="27">
+      <formula>AND($A70="end group", $B70 = "", $C70 = "", $D70 = "", $E70 = "", $F70 = "", $G70 = "", $H70 = "", $I70 = "", $J70 = "", $K70 = "", $L70 = "", $M70 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:Y70">
+    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I70">
+    <cfRule type="expression" dxfId="34" priority="29">
+      <formula>AND($I70 = "", $A70 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70">
+    <cfRule type="expression" dxfId="33" priority="30">
+      <formula>AND(AND(NOT($A70 = "end group"), NOT($A70 = "end repeat"), NOT($A70 = "")), $C70 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70">
+    <cfRule type="expression" dxfId="32" priority="31">
+      <formula>AND(AND(NOT($A70 = "end group"), NOT($A70 = "end repeat"), NOT($A70 = "")), $B70 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H70">
+    <cfRule type="expression" dxfId="30" priority="34">
+      <formula>AND(NOT($G70 = ""), $H70 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:Y70">
+    <cfRule type="expression" dxfId="29" priority="35">
+      <formula>AND($A70="begin repeat", NOT($B70 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:Y70">
+    <cfRule type="expression" dxfId="28" priority="36">
+      <formula>AND($A70="end repeat", $B70 = "", $C70 = "", $D70 = "", $E70 = "", $F70 = "", $G70 = "", $H70 = "", $I70 = "", $J70 = "", $K70 = "", $L70 = "", $M70 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="containsText" dxfId="27" priority="19" operator="containsText" text="calculate"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="expression" dxfId="26" priority="20">
+      <formula>AND($A51="begin group", NOT($B51 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="expression" dxfId="25" priority="21">
+      <formula>AND($A51="end group", $B51 = "", $C51 = "", $D51 = "", $E51 = "", $F51 = "", $G51 = "", $H51 = "", $I51 = "", $J51 = "", $K51 = "", $L51 = "", $M51 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="expression" dxfId="23" priority="23">
+      <formula>AND($A51="begin repeat", NOT($B51 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="expression" dxfId="22" priority="24">
+      <formula>AND($A51="end repeat", $B51 = "", $C51 = "", $D51 = "", $E51 = "", $F51 = "", $G51 = "", $H51 = "", $I51 = "", $J51 = "", $K51 = "", $L51 = "", $M51 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="containsText" dxfId="21" priority="13" operator="containsText" text="calculate"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="expression" dxfId="20" priority="14">
+      <formula>AND($A64="begin group", NOT($B64 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="expression" dxfId="19" priority="15">
+      <formula>AND($A64="end group", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $I64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="expression" dxfId="17" priority="17">
+      <formula>AND($A64="begin repeat", NOT($B64 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="expression" dxfId="16" priority="18">
+      <formula>AND($A64="end repeat", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $I64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="calculate"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="expression" dxfId="14" priority="2">
+      <formula>AND($A34="begin group", NOT($B34 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="expression" dxfId="13" priority="3">
+      <formula>AND($A34="end group", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>AND($I34 = "", $A34 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>AND(AND(NOT($A34 = "end group"), NOT($A34 = "end repeat"), NOT($A34 = "")), $C34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>AND(AND(NOT($A34 = "end group"), NOT($A34 = "end repeat"), NOT($A34 = "")), $B34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>AND(NOT($G34 = ""), $H34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="expression" dxfId="6" priority="10">
+      <formula>AND($A34="begin repeat", NOT($B34 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="expression" dxfId="5" priority="11">
+      <formula>AND($A34="end repeat", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B71:B986 B2:B33 B35:B69">
+    <cfRule type="expression" dxfId="4" priority="380">
+      <formula>COUNTIF($B$2:$B$986,B2)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70">
+    <cfRule type="expression" dxfId="3" priority="384">
+      <formula>COUNTIF($B$2:$B$1011,B70)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="25" priority="333">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$988, "begin group") = COUNTIF($A$1:$A$988, "end group"))</formula>
+    <cfRule type="expression" dxfId="2" priority="385">
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$987, "begin group") = COUNTIF($A$1:$A$987, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="24" priority="334">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$979, "begin group") = COUNTIF($A$1:$A$988, "end group")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="calculate"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="expression" dxfId="22" priority="20">
-      <formula>AND($A50="begin group", NOT($B50 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="expression" dxfId="21" priority="21">
-      <formula>AND($A50="end group", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="expression" dxfId="19" priority="23">
-      <formula>AND($A50="begin repeat", NOT($B50 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="expression" dxfId="18" priority="24">
-      <formula>AND($A50="end repeat", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="calculate"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
-    <cfRule type="expression" dxfId="16" priority="8">
-      <formula>AND($A70="begin group", NOT($B70 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
-    <cfRule type="expression" dxfId="15" priority="9">
-      <formula>AND($A70="end group", $B70 = "", $C70 = "", $D70 = "", $E70 = "", $F70 = "", $G70 = "", $H70 = "", $I70 = "", $J70 = "", $K70 = "", $L70 = "", $M70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="13" priority="11">
-      <formula>AND($I70 = "", $A70 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
-    <cfRule type="expression" dxfId="12" priority="12">
-      <formula>AND(AND(NOT($A70 = "end group"), NOT($A70 = "end repeat"), NOT($A70 = "")), $C70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>AND(AND(NOT($A70 = "end group"), NOT($A70 = "end repeat"), NOT($A70 = "")), $B70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>COUNTIF($B$2:$B$1012,B70)&gt;1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H70">
-    <cfRule type="expression" dxfId="8" priority="16">
-      <formula>AND(NOT($G70 = ""), $H70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
-    <cfRule type="expression" dxfId="7" priority="17">
-      <formula>AND($A70="begin repeat", NOT($B70 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
-    <cfRule type="expression" dxfId="6" priority="18">
-      <formula>AND($A70="end repeat", $B70 = "", $C70 = "", $D70 = "", $E70 = "", $F70 = "", $G70 = "", $H70 = "", $I70 = "", $J70 = "", $K70 = "", $L70 = "", $M70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="calculate"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>AND($A51="begin group", NOT($B51 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>AND($A51="end group", $B51 = "", $C51 = "", $D51 = "", $E51 = "", $F51 = "", $G51 = "", $H51 = "", $I51 = "", $J51 = "", $K51 = "", $L51 = "", $M51 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>AND($A51="begin repeat", NOT($B51 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="0" priority="6">
-      <formula>AND($A51="end repeat", $B51 = "", $C51 = "", $D51 = "", $E51 = "", $F51 = "", $G51 = "", $H51 = "", $I51 = "", $J51 = "", $K51 = "", $L51 = "", $M51 = "")</formula>
+    <cfRule type="expression" dxfId="1" priority="386">
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$978, "begin group") = COUNTIF($A$1:$A$987, "end group")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" dxfId="0" priority="387">
+      <formula>COUNTIF($B$2:$B$955,B34)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="D56:D59 D61:D66 D2:D54 D68:D77" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D56:D59 D61:D66 D2:D54 D68:D76" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4600,11 +4913,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1048557"/>
+  <dimension ref="A1:F1048563"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4631,7 +4944,7 @@
     </row>
     <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="11" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>53</v>
@@ -4642,7 +4955,7 @@
     </row>
     <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="11" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>57</v>
@@ -4651,227 +4964,381 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="1:6" ht="13.5">
+      <c r="A4" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>163</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>153</v>
+        <v>93</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="C6" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>154</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>155</v>
+        <v>93</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>156</v>
+        <v>93</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>157</v>
+        <v>93</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>56</v>
+        <v>93</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>125</v>
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>126</v>
+        <v>89</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>127</v>
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>128</v>
+      <c r="A15" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>56</v>
+      <c r="A16" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>58</v>
+        <v>126</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>56</v>
+        <v>126</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>58</v>
+        <v>127</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>137</v>
+        <v>127</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>136</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>138</v>
+        <v>129</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>139</v>
+        <v>129</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1048557" ht="15.75" customHeight="1"/>
+      <c r="C29" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="1048563" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4916,14 +5383,14 @@
     </row>
     <row r="2" spans="1:6" ht="27">
       <c r="A2" s="11" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C2" s="12">
         <f ca="1">NOW()</f>
-        <v>43999.507017245371</v>
+        <v>44000.9186162037</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>65</v>

</xml_diff>